<commit_message>
page object start update
</commit_message>
<xml_diff>
--- a/Test asperitas new.xlsx
+++ b/Test asperitas new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test_asperitas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392943E8-3EDE-4E4C-9EDA-4D878FD730A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA34AA04-7110-4F74-BDB9-C715DD853111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{50901EC0-5944-4AB6-8707-8FF3B192D060}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="70">
   <si>
     <t>Проект</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>6. Над полем регистрации появилось сообщение "INVALID PASSWORD"</t>
+  </si>
+  <si>
+    <t>3. Заполнить поле "USERNAME" - "АнтохаФролл"</t>
   </si>
 </sst>
 </file>
@@ -875,6 +878,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -904,9 +910,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1240,64 +1243,64 @@
       <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="74"/>
+      <c r="D2" s="75"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="76"/>
+      <c r="D3" s="77"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="76"/>
+      <c r="D4" s="77"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="76"/>
+      <c r="D5" s="77"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="77">
+      <c r="C6" s="78">
         <v>44916</v>
       </c>
-      <c r="D6" s="78"/>
+      <c r="D6" s="79"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="76"/>
+      <c r="D7" s="77"/>
     </row>
     <row r="8" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="71" t="s">
+      <c r="C8" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="72"/>
+      <c r="D8" s="73"/>
     </row>
     <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="28" t="s">
@@ -1320,7 +1323,7 @@
       <c r="D10" s="37"/>
     </row>
     <row r="11" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="70" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="39" t="s">
@@ -1329,77 +1332,77 @@
       <c r="D11" s="25"/>
     </row>
     <row r="12" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="69"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="40" t="s">
         <v>35</v>
       </c>
       <c r="D12" s="26"/>
     </row>
     <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="69"/>
+      <c r="B13" s="70"/>
       <c r="C13" s="40" t="s">
         <v>36</v>
       </c>
       <c r="D13" s="26"/>
     </row>
     <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="69"/>
+      <c r="B14" s="70"/>
       <c r="C14" s="40" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="26"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="69"/>
+      <c r="B15" s="70"/>
       <c r="C15" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="26"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="69"/>
+      <c r="B16" s="70"/>
       <c r="C16" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="26"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="69"/>
+      <c r="B17" s="70"/>
       <c r="C17" s="40" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="26"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="69"/>
+      <c r="B18" s="70"/>
       <c r="C18" s="40" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="26"/>
     </row>
     <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="69"/>
+      <c r="B19" s="70"/>
       <c r="C19" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D19" s="26"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="69"/>
+      <c r="B20" s="70"/>
       <c r="C20" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D20" s="6"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="69"/>
+      <c r="B21" s="70"/>
       <c r="C21" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D21" s="6"/>
     </row>
     <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="70"/>
+      <c r="B22" s="71"/>
       <c r="C22" s="22" t="s">
         <v>45</v>
       </c>
@@ -1425,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F667479D-B99A-4D84-94BD-2129C8561E96}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,9 +1927,9 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="79"/>
+      <c r="A68" s="69"/>
       <c r="B68" s="40" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="C68" s="40" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
open, signup, login done!
</commit_message>
<xml_diff>
--- a/Test asperitas new.xlsx
+++ b/Test asperitas new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test_asperitas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96BD2C9-111E-4C04-8AFC-5EE932C3F364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71346E69-5EDB-487B-B536-2CC052D20D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{50901EC0-5944-4AB6-8707-8FF3B192D060}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{50901EC0-5944-4AB6-8707-8FF3B192D060}"/>
   </bookViews>
   <sheets>
     <sheet name="Чек-лист" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="86">
   <si>
     <t>Проект</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>1. Открыт сайт https://asperitas.vercel.app/</t>
-  </si>
-  <si>
-    <t>3. Заполнить поле "USERNAME" - АнтохаФролл</t>
   </si>
   <si>
     <t>Регистрация нового пользователя с корректными данными</t>
@@ -178,10 +175,6 @@
     <t>4. Заполнить поле "USERNAME" - "AntohaFroll"
 Не заполнять поля "PASSWORD" и "CONFIRM PASSWORD"
 Нажать кнопку "SIGN UP"</t>
-  </si>
-  <si>
-    <t>5.  Заполнить поле "USERNAME" - "AntohaFroll"
-Начать заполнять поле "PASSWORD" - "q"</t>
   </si>
   <si>
     <t>6.Заполнить поля
@@ -266,9 +259,6 @@
     <t>ID.7</t>
   </si>
   <si>
-    <t>1. На сайте https://asperitas.vercel.app/ в строке поста любого поста нажать на пользователя, например "banana"</t>
-  </si>
-  <si>
     <t>1. Открыта страница с постом "Testing my new text post feature :)"</t>
   </si>
   <si>
@@ -284,15 +274,7 @@
     <t>1. Открыта страница с постами категории "MUSIC"</t>
   </si>
   <si>
-    <t>2. Вернуться на главную страницу, нажав на логотип с</t>
-  </si>
-  <si>
     <t>3. Заполнить поле "USERNAME" - "Antoha$roll"
-Нажать кнопку "LOG IN"</t>
-  </si>
-  <si>
-    <t>5.  Заполнить поле "USERNAME" - "AntohaFroll"
-Начать заполнять поле "PASSWORD" - "q"
 Нажать кнопку "LOG IN"</t>
   </si>
   <si>
@@ -304,6 +286,44 @@
 "USERNAME" - "AntohaFroll"
 "PASSWORD" - "qwerty123457"
 Нажать кнопку "LOG IN"</t>
+  </si>
+  <si>
+    <t>3. Заполнить поле "USERNAME" - Antoha$roll</t>
+  </si>
+  <si>
+    <t>5.  Заполнить поле "USERNAME" - "AntohaFroll"
+Заполнить поле "PASSWORD" - "q"
+Нажать кнопку "LOG IN"</t>
+  </si>
+  <si>
+    <t>5.  Заполнить поле "USERNAME" - "AntohaFroll"
+Заполнить поле "PASSWORD" - "q"
+Нажать кнопку "SIGN UP"</t>
+  </si>
+  <si>
+    <t>7.Заполнить поля
+"USERNAME" - "AntohaFroll"
+"PASSWORD" - "qwerty123456"
+"CONFIRM PASSWORD" - "qwerty123457"
+Нажать кнопку "SIGN UP"</t>
+  </si>
+  <si>
+    <t>7. Поле "CONFIRM PASSWORD" выделено красным, над полем появилось сообщение "PASSWORDS MUST MATCH"</t>
+  </si>
+  <si>
+    <t>2. Вернуться на главную страницу, нажав на логотип сайта</t>
+  </si>
+  <si>
+    <t>2. Открыта главная страница сайта</t>
+  </si>
+  <si>
+    <t>1. На сайте https://asperitas.vercel.app/ в строке любого поста нажать на пользователя, например "banana"</t>
+  </si>
+  <si>
+    <t>3. На сайте https://asperitas.vercel.app/ в строке любого поста нажать на категорию, например "/a/music"</t>
+  </si>
+  <si>
+    <t>3. Открыта страница с постами категории "MUSIC"</t>
   </si>
 </sst>
 </file>
@@ -336,12 +356,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="28">
@@ -721,7 +759,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -912,30 +950,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -966,6 +983,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1298,64 +1321,64 @@
       <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="81"/>
+      <c r="D2" s="74"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="83"/>
+      <c r="D3" s="76"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="76"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="83"/>
+      <c r="D5" s="76"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="84">
+      <c r="C6" s="77">
         <v>44916</v>
       </c>
-      <c r="D6" s="85"/>
+      <c r="D6" s="78"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="82" t="s">
+      <c r="C7" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="83"/>
+      <c r="D7" s="76"/>
     </row>
     <row r="8" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="72"/>
     </row>
     <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="27" t="s">
@@ -1373,93 +1396,93 @@
         <v>8</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="36"/>
     </row>
     <row r="11" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="69" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="24"/>
+    </row>
+    <row r="12" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="69"/>
+      <c r="C12" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="24"/>
-    </row>
-    <row r="12" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="76"/>
-      <c r="C12" s="39" t="s">
+      <c r="D12" s="25"/>
+    </row>
+    <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="69"/>
+      <c r="C13" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="25"/>
-    </row>
-    <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="76"/>
-      <c r="C13" s="39" t="s">
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="69"/>
+      <c r="C14" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="25"/>
-    </row>
-    <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="76"/>
-      <c r="C14" s="39" t="s">
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="69"/>
+      <c r="C15" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="39"/>
+    </row>
+    <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="69"/>
+      <c r="C16" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="69"/>
+      <c r="C17" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="69"/>
+      <c r="C18" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="69"/>
+      <c r="C19" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="25"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="76"/>
-      <c r="C15" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="39"/>
-    </row>
-    <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="76"/>
-      <c r="C16" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="25"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="76"/>
-      <c r="C17" s="39" t="s">
+      <c r="D19" s="25"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="69"/>
+      <c r="C20" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="69"/>
+      <c r="C21" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="25"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="76"/>
-      <c r="C18" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="39"/>
-    </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="76"/>
-      <c r="C19" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="25"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="76"/>
-      <c r="C20" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="76"/>
-      <c r="C21" s="39" t="s">
-        <v>40</v>
-      </c>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="77"/>
+      <c r="B22" s="70"/>
       <c r="C22" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D22" s="22"/>
     </row>
@@ -1481,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F667479D-B99A-4D84-94BD-2129C8561E96}">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,8 +1517,9 @@
     <col min="4" max="4" width="31.85546875" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="82"/>
       <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
@@ -1504,16 +1528,16 @@
       </c>
       <c r="D2" s="50"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="42" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="51"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="43" t="s">
         <v>2</v>
       </c>
@@ -1522,7 +1546,7 @@
       </c>
       <c r="D4" s="50"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="43" t="s">
         <v>3</v>
       </c>
@@ -1531,14 +1555,14 @@
       </c>
       <c r="D5" s="50"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="57"/>
       <c r="D6" s="50"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="43" t="s">
         <v>5</v>
       </c>
@@ -1547,16 +1571,16 @@
       </c>
       <c r="D7" s="50"/>
     </row>
-    <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="44" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="50"/>
     </row>
-    <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="45" t="s">
         <v>16</v>
       </c>
@@ -1565,8 +1589,8 @@
       </c>
       <c r="D9" s="50"/>
     </row>
-    <row r="10" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="69" t="s">
+    <row r="10" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="68" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="28" t="s">
@@ -1574,7 +1598,8 @@
       </c>
       <c r="D10" s="52"/>
     </row>
-    <row r="11" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="79"/>
       <c r="B11" s="46" t="s">
         <v>31</v>
       </c>
@@ -1583,13 +1608,14 @@
       </c>
       <c r="D11" s="51"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="67"/>
       <c r="C12" s="47"/>
       <c r="D12" s="51"/>
     </row>
-    <row r="13" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="82"/>
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1597,16 +1623,16 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="37" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="53"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
@@ -1614,7 +1640,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
@@ -1622,13 +1648,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="63"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
@@ -1636,15 +1662,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="64" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>16</v>
       </c>
@@ -1652,7 +1678,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="20" t="s">
         <v>17</v>
       </c>
@@ -1661,7 +1687,8 @@
       </c>
       <c r="D22" s="54"/>
     </row>
-    <row r="23" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="79"/>
       <c r="B23" s="38" t="s">
         <v>29</v>
       </c>
@@ -1670,26 +1697,27 @@
       </c>
       <c r="D23" s="47"/>
     </row>
-    <row r="24" spans="2:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="81"/>
       <c r="B24" s="40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" s="40" t="s">
         <v>30</v>
       </c>
       <c r="D24" s="47"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="48"/>
       <c r="C25" s="48"/>
       <c r="D25" s="47"/>
     </row>
-    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="66"/>
       <c r="C26" s="66"/>
       <c r="D26" s="47"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1697,23 +1725,23 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="37" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="61" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="62" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>3</v>
       </c>
@@ -1721,13 +1749,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="63"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>5</v>
       </c>
@@ -1735,15 +1763,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="64" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>16</v>
       </c>
@@ -1751,7 +1779,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="20" t="s">
         <v>17</v>
       </c>
@@ -1759,7 +1787,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="79"/>
       <c r="B36" s="38" t="s">
         <v>29</v>
       </c>
@@ -1767,504 +1796,527 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="79"/>
       <c r="B37" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="79"/>
+      <c r="B38" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="79"/>
+      <c r="B39" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="39" t="s">
+      <c r="C39" s="25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="39" t="s">
+    <row r="40" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="79"/>
+      <c r="B40" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B39" s="25" t="s">
+    <row r="41" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="79"/>
+      <c r="B41" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C41" s="25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B40" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="25" t="s">
+    <row r="42" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="79"/>
+      <c r="B42" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="82"/>
+      <c r="B45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="60" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="62" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="63"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="62" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="64" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="65" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="79"/>
+      <c r="B54" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" s="38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="79"/>
+      <c r="B55" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="82"/>
+      <c r="B58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="60" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="61" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="62" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="63"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="62" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="64" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="65" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="79"/>
+      <c r="B67" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C67" s="38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="79"/>
+      <c r="B68" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68" s="39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="80"/>
+      <c r="B69" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69" s="39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="79"/>
+      <c r="B70" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="79"/>
+      <c r="B71" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71" s="25" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="2:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" s="26" t="s">
+    <row r="72" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="79"/>
+      <c r="B72" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72" s="26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
+    <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="60" t="s">
+      <c r="C75" s="60" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="37" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="39" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C46" s="62" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="62" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" s="63"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="62" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="64" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="65" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" s="23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="C53" s="38" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="C54" s="40" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="60" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58" s="61" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C59" s="62" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" s="62" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61" s="63"/>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="62" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C63" s="64" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="65" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" s="23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="C66" s="38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B67" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="C67" s="39" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="68"/>
-      <c r="B68" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C68" s="39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B69" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C69" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B70" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C70" s="25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C71" s="26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C74" s="60" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C75" s="61" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C76" s="62" t="s">
-        <v>62</v>
+      <c r="C76" s="61" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C77" s="62" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C78" s="63"/>
+        <v>3</v>
+      </c>
+      <c r="C78" s="62" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="63"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C79" s="62" t="s">
+      <c r="C80" s="62" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="34" t="s">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C80" s="64" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="3" t="s">
+      <c r="C81" s="64" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C81" s="65" t="s">
+      <c r="C82" s="65" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="20" t="s">
+    <row r="83" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C82" s="23" t="s">
+      <c r="C83" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="35" t="s">
+    <row r="84" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C84" s="35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C87" s="60" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="61" t="s">
         <v>66</v>
-      </c>
-      <c r="C83" s="35" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C86" s="60" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B87" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C87" s="61" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C88" s="62" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C89" s="62" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C90" s="63"/>
+        <v>3</v>
+      </c>
+      <c r="C90" s="62" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="63"/>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C91" s="62" t="s">
+      <c r="C92" s="62" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="34" t="s">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C92" s="64" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="3" t="s">
+      <c r="C93" s="64" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C93" s="65" t="s">
+      <c r="C94" s="65" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="20" t="s">
+    <row r="95" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C94" s="23" t="s">
+      <c r="C95" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="C95" s="35" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="1" t="s">
+    <row r="96" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C96" s="35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C98" s="60" t="s">
+      <c r="C99" s="60" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="37" t="s">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C99" s="61" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C100" s="62" t="s">
-        <v>73</v>
+      <c r="C100" s="61" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C101" s="62" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C102" s="63"/>
+        <v>3</v>
+      </c>
+      <c r="C102" s="62" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C103" s="63"/>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="62" t="s">
+      <c r="C104" s="62" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="34" t="s">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B105" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C104" s="64" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="3" t="s">
+      <c r="C105" s="64" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C105" s="65" t="s">
+      <c r="C106" s="65" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="106" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="20" t="s">
+    <row r="107" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C106" s="23" t="s">
+      <c r="C107" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B107" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="C107" s="71" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="72" t="s">
-        <v>76</v>
-      </c>
-      <c r="C108" s="73" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="109" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="C109" s="75" t="s">
-        <v>75</v>
+    <row r="108" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B108" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C108" s="38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B109" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C109" s="39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B110" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C110" s="40" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
post page in work
</commit_message>
<xml_diff>
--- a/Test asperitas new.xlsx
+++ b/Test asperitas new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test_asperitas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D19D4F9-AB13-4CA1-B0C3-F71A862892B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02266408-CA9B-472D-8850-8C1206F0C53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{50901EC0-5944-4AB6-8707-8FF3B192D060}"/>
   </bookViews>
@@ -1086,59 +1086,59 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1679,8 +1679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F667479D-B99A-4D84-94BD-2129C8561E96}">
   <dimension ref="A1:D204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A134" sqref="A134"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D141" sqref="D141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2705,6 +2705,7 @@
       </c>
     </row>
     <row r="141" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="56"/>
       <c r="B141" s="27" t="s">
         <v>101</v>
       </c>
@@ -3177,56 +3178,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="109" t="s">
+      <c r="C2" s="116"/>
+      <c r="D2" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="109"/>
+      <c r="E2" s="110"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="110" t="s">
+      <c r="C3" s="112"/>
+      <c r="D3" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="110"/>
+      <c r="E3" s="111"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="110" t="s">
+      <c r="C5" s="112"/>
+      <c r="D5" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="110"/>
+      <c r="E5" s="111"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="111" t="s">
+      <c r="C6" s="114"/>
+      <c r="D6" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="111"/>
+      <c r="E6" s="113"/>
     </row>
     <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="77" t="s">
@@ -3269,52 +3270,52 @@
       <c r="E10" s="81"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="107" t="s">
+      <c r="B11" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="108"/>
-      <c r="D11" s="101" t="s">
+      <c r="C11" s="107"/>
+      <c r="D11" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="102"/>
+      <c r="E11" s="109"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="104"/>
-      <c r="D12" s="105" t="s">
+      <c r="C12" s="99"/>
+      <c r="D12" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="E12" s="106"/>
+      <c r="E12" s="101"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="104"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="104"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="99"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="103" t="s">
+      <c r="B14" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="104"/>
-      <c r="D14" s="105" t="s">
+      <c r="C14" s="99"/>
+      <c r="D14" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="106"/>
+      <c r="E14" s="101"/>
     </row>
     <row r="15" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="113" t="s">
+      <c r="B15" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="114"/>
-      <c r="D15" s="115" t="s">
+      <c r="C15" s="103"/>
+      <c r="D15" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="116"/>
+      <c r="E15" s="105"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="77" t="s">
@@ -3360,52 +3361,52 @@
     </row>
     <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="107" t="s">
+      <c r="B21" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="108"/>
-      <c r="D21" s="101" t="s">
+      <c r="C21" s="107"/>
+      <c r="D21" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="102"/>
+      <c r="E21" s="109"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="105" t="s">
+      <c r="C22" s="99"/>
+      <c r="D22" s="100" t="s">
         <v>139</v>
       </c>
-      <c r="E22" s="106"/>
+      <c r="E22" s="101"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="103" t="s">
+      <c r="B23" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="104"/>
-      <c r="D23" s="103"/>
-      <c r="E23" s="104"/>
+      <c r="C23" s="99"/>
+      <c r="D23" s="98"/>
+      <c r="E23" s="99"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="103" t="s">
+      <c r="B24" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="104"/>
-      <c r="D24" s="105" t="s">
+      <c r="C24" s="99"/>
+      <c r="D24" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="106"/>
+      <c r="E24" s="101"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="113" t="s">
+      <c r="B25" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="114"/>
-      <c r="D25" s="115" t="s">
+      <c r="C25" s="103"/>
+      <c r="D25" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="116"/>
+      <c r="E25" s="105"/>
     </row>
     <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="77" t="s">
@@ -3451,52 +3452,52 @@
     </row>
     <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="107" t="s">
+      <c r="B31" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="108"/>
-      <c r="D31" s="101" t="s">
+      <c r="C31" s="107"/>
+      <c r="D31" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="E31" s="102"/>
+      <c r="E31" s="109"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="103" t="s">
+      <c r="B32" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="104"/>
-      <c r="D32" s="105" t="s">
+      <c r="C32" s="99"/>
+      <c r="D32" s="100" t="s">
         <v>142</v>
       </c>
-      <c r="E32" s="106"/>
+      <c r="E32" s="101"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="103" t="s">
+      <c r="B33" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="104"/>
-      <c r="D33" s="103"/>
-      <c r="E33" s="104"/>
+      <c r="C33" s="99"/>
+      <c r="D33" s="98"/>
+      <c r="E33" s="99"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="103" t="s">
+      <c r="B34" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="104"/>
-      <c r="D34" s="105" t="s">
+      <c r="C34" s="99"/>
+      <c r="D34" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="106"/>
+      <c r="E34" s="101"/>
     </row>
     <row r="35" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="113" t="s">
+      <c r="B35" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="114"/>
-      <c r="D35" s="115" t="s">
+      <c r="C35" s="103"/>
+      <c r="D35" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="116"/>
+      <c r="E35" s="105"/>
     </row>
     <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="77" t="s">
@@ -3598,52 +3599,52 @@
     </row>
     <row r="44" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="107" t="s">
+      <c r="B45" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="108"/>
-      <c r="D45" s="101" t="s">
+      <c r="C45" s="107"/>
+      <c r="D45" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="102"/>
+      <c r="E45" s="109"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="103" t="s">
+      <c r="B46" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="104"/>
-      <c r="D46" s="105" t="s">
+      <c r="C46" s="99"/>
+      <c r="D46" s="100" t="s">
         <v>148</v>
       </c>
-      <c r="E46" s="106"/>
+      <c r="E46" s="101"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="103" t="s">
+      <c r="B47" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="104"/>
-      <c r="D47" s="103"/>
-      <c r="E47" s="104"/>
+      <c r="C47" s="99"/>
+      <c r="D47" s="98"/>
+      <c r="E47" s="99"/>
     </row>
     <row r="48" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="103" t="s">
+      <c r="B48" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="104"/>
-      <c r="D48" s="105" t="s">
+      <c r="C48" s="99"/>
+      <c r="D48" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="106"/>
+      <c r="E48" s="101"/>
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="113" t="s">
+      <c r="B49" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C49" s="114"/>
-      <c r="D49" s="115" t="s">
+      <c r="C49" s="103"/>
+      <c r="D49" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="E49" s="116"/>
+      <c r="E49" s="105"/>
     </row>
     <row r="50" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="77" t="s">
@@ -3721,42 +3722,11 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:E12"/>
@@ -3767,11 +3737,42 @@
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>